<commit_message>
series of logistic regressions for response at each split
</commit_message>
<xml_diff>
--- a/results/d20_JN.xlsx
+++ b/results/d20_JN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmm5708.PSU\Documents\hannah-merseal\jazznets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmm5708.PSU\Documents\hannah-merseal\jazznets\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{032D6752-D115-42DA-B567-BBCD04CBB443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F18F8A-59FE-49C3-9D00-C3BA0D6B563F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{889ACF90-31BA-4362-B15B-D8BE58B2A8A8}"/>
+    <workbookView xWindow="-38700" yWindow="1545" windowWidth="19425" windowHeight="10620" xr2:uid="{889ACF90-31BA-4362-B15B-D8BE58B2A8A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678FD4DB-9968-4F94-9F24-8EE6DA8516BB}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,7 +552,7 @@
         <v>69.827586206896598</v>
       </c>
       <c r="I3" s="5">
-        <v>45.909614718604999</v>
+        <v>69.827586206896598</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -581,7 +581,7 @@
         <v>63.557993730407503</v>
       </c>
       <c r="I4" s="5">
-        <v>48.136148123274097</v>
+        <v>63.557993730407503</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -610,7 +610,7 @@
         <v>56.198347107437996</v>
       </c>
       <c r="I5" s="5">
-        <v>49.6240830576658</v>
+        <v>56.198347107437996</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -639,7 +639,7 @@
         <v>50.236034618410699</v>
       </c>
       <c r="I6" s="5">
-        <v>50.009280442271695</v>
+        <v>50.236034618410699</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>